<commit_message>
v2.1.5 fix a lot of bugs
</commit_message>
<xml_diff>
--- a/Duty/График дежурств 7 этаж.xlsx
+++ b/Duty/График дежурств 7 этаж.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\PycharmProjects\Bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\PycharmProjects\Bot\Duty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9414EE-7E16-4763-8B2E-1AEF38838F6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308E7E8A-C14E-4F32-BB07-942C7FD75E76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>ГРАФИК ДЕЖУРСТВ ПО ЭТАЖУ</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>Сметанкина</t>
-  </si>
-  <si>
-    <t>Маликова</t>
   </si>
   <si>
     <t>Юсупова</t>
@@ -707,8 +704,8 @@
   </sheetPr>
   <dimension ref="A1:AY999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1190,7 @@
     </row>
     <row r="10" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="12">
         <v>713</v>
@@ -1273,7 +1270,7 @@
     </row>
     <row r="12" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="12">
         <v>702</v>
@@ -2100,7 +2097,7 @@
     </row>
     <row r="31" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B31" s="12">
         <v>714</v>
@@ -2149,7 +2146,7 @@
     </row>
     <row r="32" spans="1:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="12">
         <v>714</v>
@@ -2198,7 +2195,7 @@
     </row>
     <row r="33" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="12">
         <v>712</v>
@@ -2250,15 +2247,15 @@
     </row>
     <row r="35" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH35" s="52" t="s">
         <v>31</v>
-      </c>
-      <c r="AH35" s="52" t="s">
-        <v>32</v>
       </c>
       <c r="AI35" s="43"/>
       <c r="AJ35" s="43"/>
       <c r="AM35" s="42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AN35" s="43"/>
       <c r="AO35" s="43"/>
@@ -2267,13 +2264,13 @@
     </row>
     <row r="36" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AH36" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AI36" s="43"/>
       <c r="AJ36" s="43"/>
       <c r="AK36" s="2"/>
       <c r="AM36" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AN36" s="43"/>
       <c r="AO36" s="43"/>

</xml_diff>